<commit_message>
Madhuri Ghute changes in order management
</commit_message>
<xml_diff>
--- a/WebApp/admin/public/BulkUploadTemplates/Finish Goods Inward Template.xlsx
+++ b/WebApp/admin/public/BulkUploadTemplates/Finish Goods Inward Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -39,9 +39,6 @@
     <t>fgTotalQty</t>
   </si>
   <si>
-    <t>fgUnitQtyforFG</t>
-  </si>
-  <si>
     <t>finishedGoodsUnit</t>
   </si>
   <si>
@@ -64,12 +61,6 @@
   </si>
   <si>
     <t>Madhuri</t>
-  </si>
-  <si>
-    <t>fgInwardQty</t>
-  </si>
-  <si>
-    <t>fgInwardUnit</t>
   </si>
   <si>
     <t>Chikku</t>
@@ -418,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,18 +420,17 @@
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="2" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1"/>
-    <col min="12" max="12" width="21" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" customWidth="1"/>
-    <col min="16" max="16" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,10 +438,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -460,45 +450,36 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44007</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>2160</v>
@@ -507,37 +488,28 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
         <v>100</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2">
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2">
-        <v>100</v>
-      </c>
-      <c r="L2">
-        <v>100</v>
+      <c r="L2" t="s">
+        <v>13</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Madhuri Ghute changes in Inventory management
</commit_message>
<xml_diff>
--- a/WebApp/admin/public/BulkUploadTemplates/Finish Goods Inward Template.xlsx
+++ b/WebApp/admin/public/BulkUploadTemplates/Finish Goods Inward Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>FR106</t>
+  </si>
+  <si>
+    <t>finishedGoodsTotalQty</t>
   </si>
 </sst>
 </file>
@@ -409,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,14 +426,14 @@
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.140625" customWidth="1"/>
-    <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="32.140625" customWidth="1"/>
+    <col min="9" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,21 +462,24 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>44007</v>
+        <v>44037</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -499,16 +505,19 @@
       <c r="I2">
         <v>100</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>